<commit_message>
cap nhat bai tap
</commit_message>
<xml_diff>
--- a/tuan 2.xlsx
+++ b/tuan 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dai hoc\kinh te cong nghe phan mem\tuần 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69338213-B957-4E74-BBC3-946C6F2C1011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C1C80A-4611-4FAA-A889-4602D639E269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="873" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="873" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="điểm actors" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -574,9 +574,9 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,19 +614,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -675,42 +662,48 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -774,146 +767,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1035,7 +888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1075,148 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,9 +941,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1241,157 +1015,199 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="14" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1675,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E167C00-17FB-45CD-BE54-4E4026166B14}">
-  <dimension ref="A3:G8"/>
+  <dimension ref="A4:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1691,115 +1507,115 @@
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="75" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>1</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="99">
         <v>0</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <v>1</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="18">
         <f>D5*E5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="99">
         <v>0</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <v>2</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="18">
         <f>D6*E6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>3</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="99">
         <v>7</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="18">
         <v>3</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="18">
         <f>D7*E7</f>
         <v>21</v>
       </c>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>4</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="98">
         <f>SUM(F5:F7)</f>
         <v>21</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="16"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="OlhSxVP/XcCs0xya95IJ6n+ijJbtJZWhHKIyiraRXOwTKpZ+KMlahCVgJKXYYtOJHFBu6op2yX0sXTDRlpXyww==" saltValue="1SllMtd0TV57h1AmmngXOQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1807,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC348462-0C24-4228-8A9B-1AFA4E502652}">
-  <dimension ref="B3:H17"/>
+  <dimension ref="B4:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,273 +1640,282 @@
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="2:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="77" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="27">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="47">
         <v>1</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="29">
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="10">
+        <f>SUM(F6:F8)</f>
+        <v>205</v>
+      </c>
+      <c r="G5" s="90">
         <f>SUM(G6:G8)</f>
         <v>1065</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="50" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31"/>
-      <c r="C6" s="32" t="s">
+    <row r="6" spans="2:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="51"/>
+      <c r="C6" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="53">
         <v>5</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="54">
         <v>1</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="100">
         <v>197</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="54">
         <f>PRODUCT(D6:F6)</f>
         <v>985</v>
       </c>
-      <c r="H6" s="60"/>
-    </row>
-    <row r="7" spans="2:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="31"/>
-      <c r="C7" s="32" t="s">
+      <c r="H6" s="50"/>
+    </row>
+    <row r="7" spans="2:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="51"/>
+      <c r="C7" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="53">
         <v>10</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="54">
         <v>1</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="100">
         <v>8</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="54">
         <f t="shared" ref="G7:G8" si="0">PRODUCT(D7:F7)</f>
         <v>80</v>
       </c>
-      <c r="H7" s="60"/>
-    </row>
-    <row r="8" spans="2:8" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31"/>
-      <c r="C8" s="32" t="s">
+      <c r="H7" s="50"/>
+    </row>
+    <row r="8" spans="2:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="51"/>
+      <c r="C8" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="53">
         <v>15</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="54">
         <v>1</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="100">
         <v>0</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="61"/>
-    </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="35">
+      <c r="H8" s="50"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="47">
         <v>2</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38">
+      <c r="D9" s="10"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="10">
+        <f>SUM(F10:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="90">
         <f>SUM(G10:G12)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="62" t="s">
+      <c r="H9" s="50" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="39"/>
-      <c r="C10" s="40" t="s">
+    <row r="10" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
+      <c r="C10" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="53">
         <v>5</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="100">
         <v>0</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="H10" s="60"/>
-    </row>
-    <row r="11" spans="2:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="39"/>
-      <c r="C11" s="32" t="s">
+      <c r="H10" s="50"/>
+    </row>
+    <row r="11" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="51"/>
+      <c r="C11" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="53">
         <v>10</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="100">
         <v>0</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="H11" s="60"/>
-    </row>
-    <row r="12" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="39"/>
-      <c r="C12" s="32" t="s">
+      <c r="H11" s="50"/>
+    </row>
+    <row r="12" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="51"/>
+      <c r="C12" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="53">
         <v>15</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="100">
         <v>0</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="61"/>
-    </row>
-    <row r="13" spans="2:8" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="43">
+      <c r="H12" s="50"/>
+    </row>
+    <row r="13" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="47">
         <v>3</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38">
+      <c r="D13" s="10"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="10">
+        <f>SUM(F14:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="90">
         <f>SUM(G14:G16)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="62" t="s">
+      <c r="H13" s="50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="39"/>
-      <c r="C14" s="40" t="s">
+    <row r="14" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
+      <c r="C14" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="53">
         <v>5</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="100">
         <v>0</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="60"/>
-    </row>
-    <row r="15" spans="2:8" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="39"/>
-      <c r="C15" s="32" t="s">
+      <c r="H14" s="50"/>
+    </row>
+    <row r="15" spans="2:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51"/>
+      <c r="C15" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="53">
         <v>10</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="100">
         <v>0</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="60"/>
-    </row>
-    <row r="16" spans="2:8" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="39"/>
-      <c r="C16" s="32" t="s">
+      <c r="H15" s="50"/>
+    </row>
+    <row r="16" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
+      <c r="C16" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="53">
         <v>15</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="100">
         <v>0</v>
       </c>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="61"/>
-    </row>
-    <row r="17" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="44"/>
-      <c r="C17" s="28" t="s">
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" spans="2:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="51"/>
+      <c r="C17" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="29">
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="90">
         <f>SUM(G5+G9+G13)</f>
         <v>1065</v>
       </c>
-      <c r="H17" s="45"/>
+      <c r="H17" s="55"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="xGH+z9xhnfSCKw9dy9+r5IvYAjHmihhp/A9DOwx6ykEQoQvIoR+/XqpEIaKKYD5ORqA5BACKoTADM4E1Del5SQ==" saltValue="m2ygUvYwwAt2DZRytfajtQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="H5:H8"/>
     <mergeCell ref="H9:H12"/>
@@ -2104,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDAD77E-15D1-450C-B2F9-CA241A131530}">
   <dimension ref="B4:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2118,313 +1943,314 @@
     <col min="7" max="7" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="107" t="s">
+    <row r="4" spans="2:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="108" t="s">
+      <c r="F4" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="108" t="s">
+      <c r="G4" s="79" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="109"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="2:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="109">
+      <c r="B6" s="24">
         <v>1</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="112">
+      <c r="D6" s="27">
         <v>2</v>
       </c>
-      <c r="E6" s="113">
+      <c r="E6" s="101">
         <v>1</v>
       </c>
-      <c r="F6" s="109">
+      <c r="F6" s="24">
         <f>PRODUCT(D6:E6)</f>
         <v>2</v>
       </c>
-      <c r="G6" s="109"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="2:7" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="109">
+      <c r="B7" s="24">
         <v>2</v>
       </c>
-      <c r="C7" s="111" t="s">
+      <c r="C7" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="112">
+      <c r="D7" s="27">
         <v>1</v>
       </c>
-      <c r="E7" s="113">
+      <c r="E7" s="101">
         <v>2</v>
       </c>
-      <c r="F7" s="109">
+      <c r="F7" s="24">
         <f t="shared" ref="F7:F16" si="0">PRODUCT(D7:E7)</f>
         <v>2</v>
       </c>
-      <c r="G7" s="109"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="2:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="109">
+      <c r="B8" s="24">
         <v>3</v>
       </c>
-      <c r="C8" s="111" t="s">
+      <c r="C8" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="112">
+      <c r="D8" s="27">
         <v>1</v>
       </c>
-      <c r="E8" s="113">
+      <c r="E8" s="101">
         <v>2</v>
       </c>
-      <c r="F8" s="109">
+      <c r="F8" s="24">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G8" s="109"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="2:7" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="109">
+      <c r="B9" s="24">
         <v>4</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="112">
+      <c r="D9" s="27">
         <v>1</v>
       </c>
-      <c r="E9" s="113">
+      <c r="E9" s="101">
         <v>2</v>
       </c>
-      <c r="F9" s="109">
+      <c r="F9" s="24">
         <f>PRODUCT(D9:E9)</f>
         <v>2</v>
       </c>
-      <c r="G9" s="109"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="109">
+      <c r="B10" s="24">
         <v>5</v>
       </c>
-      <c r="C10" s="111" t="s">
+      <c r="C10" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="112">
+      <c r="D10" s="27">
         <v>1</v>
       </c>
-      <c r="E10" s="113">
+      <c r="E10" s="101">
         <v>1</v>
       </c>
-      <c r="F10" s="109">
+      <c r="F10" s="24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="109"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="109">
+      <c r="B11" s="24">
         <v>6</v>
       </c>
-      <c r="C11" s="111" t="s">
+      <c r="C11" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="112">
+      <c r="D11" s="27">
         <v>0.5</v>
       </c>
-      <c r="E11" s="113">
+      <c r="E11" s="101">
         <v>1</v>
       </c>
-      <c r="F11" s="109">
+      <c r="F11" s="24">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G11" s="109"/>
-    </row>
-    <row r="12" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="109">
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="2:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="24">
         <v>7</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="112">
+      <c r="D12" s="27">
         <v>0.5</v>
       </c>
-      <c r="E12" s="113">
+      <c r="E12" s="101">
         <v>1</v>
       </c>
-      <c r="F12" s="109">
+      <c r="F12" s="24">
         <f>PRODUCT(D12:E12)</f>
         <v>0.5</v>
       </c>
-      <c r="G12" s="109"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="2:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="109">
+      <c r="B13" s="24">
         <v>8</v>
       </c>
-      <c r="C13" s="111" t="s">
+      <c r="C13" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="112">
+      <c r="D13" s="27">
         <v>2</v>
       </c>
-      <c r="E13" s="113">
+      <c r="E13" s="101">
         <v>1</v>
       </c>
-      <c r="F13" s="109">
+      <c r="F13" s="24">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G13" s="109"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="109">
+      <c r="B14" s="24">
         <v>9</v>
       </c>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="112">
+      <c r="D14" s="27">
         <v>1</v>
       </c>
-      <c r="E14" s="113">
+      <c r="E14" s="101">
         <v>2</v>
       </c>
-      <c r="F14" s="109">
+      <c r="F14" s="24">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="109"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="2:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="109">
+      <c r="B15" s="24">
         <v>10</v>
       </c>
-      <c r="C15" s="111" t="s">
+      <c r="C15" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="112">
+      <c r="D15" s="27">
         <v>1</v>
       </c>
-      <c r="E15" s="113">
+      <c r="E15" s="101">
         <v>2</v>
       </c>
-      <c r="F15" s="109">
+      <c r="F15" s="24">
         <f>PRODUCT(D15:E15)</f>
         <v>2</v>
       </c>
-      <c r="G15" s="109"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="109">
+      <c r="B16" s="24">
         <v>11</v>
       </c>
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="112">
+      <c r="D16" s="27">
         <v>1</v>
       </c>
-      <c r="E16" s="113">
+      <c r="E16" s="101">
         <v>1</v>
       </c>
-      <c r="F16" s="109">
+      <c r="F16" s="24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G16" s="109"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="2:7" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="109">
+      <c r="B17" s="24">
         <v>12</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="112">
+      <c r="D17" s="27">
         <v>1</v>
       </c>
-      <c r="E17" s="113">
+      <c r="E17" s="101">
         <v>2</v>
       </c>
-      <c r="F17" s="109">
+      <c r="F17" s="24">
         <f>PRODUCT(D17:E17)</f>
         <v>2</v>
       </c>
-      <c r="G17" s="109"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="109">
+      <c r="B18" s="24">
         <v>13</v>
       </c>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="112">
+      <c r="D18" s="27">
         <v>1</v>
       </c>
-      <c r="E18" s="113" t="s">
+      <c r="E18" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="F18" s="109">
+      <c r="F18" s="24">
         <v>0</v>
       </c>
-      <c r="G18" s="109"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C19" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="107">
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="91">
         <f>SUM(F6:F18)</f>
         <v>19</v>
       </c>
-      <c r="G19" s="109"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="114"/>
-      <c r="C20" s="115" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="116">
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="92">
         <f>0.6+(0.01*F19)</f>
         <v>0.79</v>
       </c>
-      <c r="G20" s="114"/>
+      <c r="G20" s="28"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="xujtfyW62X3Q7hfakz4BsBsmO7Ee69bsZXrkWsPwH/QisfePlAe1fg/aX+eU01ooqtRLgtM9iVt3gutwlamf5Q==" saltValue="MSVIgR7cjVOfhN9wsiFOKw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="C20:E20"/>
   </mergeCells>
@@ -2436,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A22" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2452,28 +2278,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="74" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2485,442 +2311,442 @@
         <v>9</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="63">
+      <c r="A4" s="34">
         <v>1</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="32">
         <v>1.5</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="102">
         <v>3</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="33">
         <f>E4*D4</f>
         <v>4.5</v>
       </c>
-      <c r="G4" s="65" t="str" cm="1">
+      <c r="G4" s="32" t="str" cm="1">
         <f t="array" ref="G4">_xlfn.IFS(F4&gt;3,"1",F4&gt;2,"0.6",F4&gt;1,"0.1",F4&gt;0,"0.05",F4&lt;=0,"0")</f>
         <v>1</v>
       </c>
-      <c r="H4" s="65"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="9" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="63">
+      <c r="A7" s="34">
         <v>2</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="32">
         <v>0.5</v>
       </c>
-      <c r="E7" s="65">
+      <c r="E7" s="102">
         <v>3</v>
       </c>
-      <c r="F7" s="67">
+      <c r="F7" s="33">
         <f>E7*D7</f>
         <v>1.5</v>
       </c>
-      <c r="G7" s="65" t="str" cm="1">
+      <c r="G7" s="32" t="str" cm="1">
         <f t="array" ref="G7">_xlfn.IFS(F7&gt;3,"1",F7&gt;2,"0.6",F7&gt;1,"0.1",F7&gt;0,"0.05",F7&lt;=0,"0")</f>
         <v>0.1</v>
       </c>
-      <c r="H7" s="66"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="63"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="66"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63">
+      <c r="A10" s="34">
         <v>3</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="32">
         <v>1</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="102">
         <v>3</v>
       </c>
-      <c r="F10" s="67">
+      <c r="F10" s="33">
         <f>E10*D10</f>
         <v>3</v>
       </c>
-      <c r="G10" s="65" t="str" cm="1">
+      <c r="G10" s="32" t="str" cm="1">
         <f t="array" ref="G10">_xlfn.IFS(F10&gt;3,"1",F10&gt;2,"0.6",F10&gt;1,"0.1",F10&gt;0,"0.05",F10&lt;=0,"0")</f>
         <v>0.6</v>
       </c>
-      <c r="H10" s="66"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="66"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="31"/>
     </row>
     <row r="12" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="66"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="31"/>
     </row>
     <row r="13" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63">
+      <c r="A13" s="34">
         <v>4</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="32">
         <v>0.5</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="102">
         <v>3</v>
       </c>
-      <c r="F13" s="67">
+      <c r="F13" s="33">
         <f>E13*D13</f>
         <v>1.5</v>
       </c>
-      <c r="G13" s="65" t="str" cm="1">
+      <c r="G13" s="32" t="str" cm="1">
         <f t="array" ref="G13">_xlfn.IFS(F13&gt;3,"1",F13&gt;2,"0.6",F13&gt;1,"0.1",F13&gt;0,"0.05",F13&lt;=0,"0")</f>
         <v>0.1</v>
       </c>
-      <c r="H13" s="66"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="9" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63">
+      <c r="A16" s="34">
         <v>5</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="32">
         <v>1</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="102">
         <v>3</v>
       </c>
-      <c r="F16" s="67">
+      <c r="F16" s="33">
         <f>E16*D16</f>
         <v>3</v>
       </c>
-      <c r="G16" s="65" t="str" cm="1">
+      <c r="G16" s="32" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.IFS(F16&gt;3,"1",F16&gt;2,"0.6",F16&gt;1,"0.1",F16&gt;0,"0.05",F16&lt;=0,"0")</f>
         <v>0.6</v>
       </c>
-      <c r="H16" s="66"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="66"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="9" t="s">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="10"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="103"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="63">
+      <c r="A20" s="34">
         <v>6</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="32">
         <v>2</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="104">
         <v>3</v>
       </c>
-      <c r="F20" s="66">
+      <c r="F20" s="31">
         <f>E20*D20</f>
         <v>6</v>
       </c>
-      <c r="G20" s="66" t="str" cm="1">
+      <c r="G20" s="31" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.IFS(F20&gt;3,"1",F20&gt;2,"0.6",F20&gt;1,"0.1",F20&gt;0,"0.05",F20&lt;=0,"0")</f>
         <v>1</v>
       </c>
-      <c r="H20" s="66"/>
+      <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="9" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="65"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63">
+      <c r="A22" s="34">
         <v>7</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="32">
         <v>-1</v>
       </c>
-      <c r="E22" s="66">
+      <c r="E22" s="104">
         <v>0</v>
       </c>
-      <c r="F22" s="66">
+      <c r="F22" s="31">
         <f>E22*D22</f>
         <v>0</v>
       </c>
-      <c r="G22" s="66" t="str" cm="1">
+      <c r="G22" s="31" t="str" cm="1">
         <f t="array" ref="G22">_xlfn.IFS(F22&gt;3,"1",F22&gt;2,"0.6",F22&gt;1,"0.1",F22&gt;0,"0.05",F22&lt;=0,"0")</f>
         <v>0</v>
       </c>
-      <c r="H22" s="66"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="34"/>
+      <c r="B23" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
     </row>
     <row r="24" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="9" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
     </row>
     <row r="25" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="63">
+      <c r="A25" s="34">
         <v>8</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="32">
         <v>-1</v>
       </c>
-      <c r="E25" s="66">
+      <c r="E25" s="104">
         <v>3</v>
       </c>
-      <c r="F25" s="66">
+      <c r="F25" s="31">
         <f>E25*D25</f>
         <v>-3</v>
       </c>
-      <c r="G25" s="66" t="str" cm="1">
+      <c r="G25" s="31" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.IFS(F25&gt;3,"1",F25&gt;2,"0.6",F25&gt;1,"0.1",F25&gt;0,"0.05",F25&lt;=0,"0")</f>
         <v>0</v>
       </c>
-      <c r="H25" s="66"/>
+      <c r="H25" s="31"/>
     </row>
     <row r="26" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="9" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="65"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="9" t="s">
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
     </row>
     <row r="28" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="14">
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="93">
         <f>SUM(F4:F27)</f>
         <v>16.5</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
     </row>
     <row r="29" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -2932,14 +2758,14 @@
       <c r="C29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="14">
+      <c r="D29" s="62"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="93">
         <f>1.4+(-0.03*F28)</f>
         <v>0.90499999999999992</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
     </row>
     <row r="30" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
@@ -2951,14 +2777,14 @@
       <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="14">
+      <c r="D30" s="62"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="93">
         <f>G4+G7+G10+G13+G16+G20+G22+G25</f>
         <v>3.4000000000000004</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="64"/>
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
@@ -2970,33 +2796,41 @@
       <c r="C31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="14" t="str" cm="1">
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="93" t="str" cm="1">
         <f t="array" ref="G31">_xlfn.IFS(G30&gt;=3,"20", G30&gt;1,"32",G30 &lt;1,"48")</f>
         <v>20</v>
       </c>
-      <c r="H31" s="6"/>
+      <c r="H31" s="64"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="34S14NYKldJVHoZP5QOH0G7lZA8/NfA7ajFJ/CD9/1i2+oIOJVMMOJoZ7c8WgZLwkXjwJrbSIb57YyKtGWiBkQ==" saltValue="/Sz56hQhPf1M+HhlpkELhg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="55">
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="G22:G24"/>
     <mergeCell ref="G25:G27"/>
     <mergeCell ref="H4:H6"/>
@@ -3013,29 +2847,22 @@
     <mergeCell ref="G13:G15"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3046,252 +2873,253 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B98F674-A8AD-4DF9-917D-D4784F6AB6B0}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="95" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="96" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="95" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="95" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" style="95" customWidth="1"/>
-    <col min="6" max="6" width="22" style="104" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="95" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="95"/>
+    <col min="1" max="1" width="11" style="57" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="56" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="57" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="57" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="22" style="61" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="57"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F2" s="97" t="s">
+    <row r="2" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="F2" s="58" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="98" t="s">
+    <row r="4" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="99" t="s">
+      <c r="E4" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="80" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="98" t="s">
+    <row r="5" spans="2:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="99" t="s">
+      <c r="C5" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="98"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="100">
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="59"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="101"/>
-      <c r="E6" s="102">
+      <c r="D6" s="10"/>
+      <c r="E6" s="88">
         <f>'điểm actors'!F8</f>
         <v>21</v>
       </c>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="100">
+    <row r="7" spans="2:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="101"/>
-      <c r="E7" s="102">
+      <c r="D7" s="10"/>
+      <c r="E7" s="88">
         <f>'Bang tinh diem Use-case'!G17</f>
         <v>1065</v>
       </c>
-      <c r="F7" s="100" t="s">
+      <c r="F7" s="19" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="100">
+    <row r="8" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C8" s="101" t="s">
+      <c r="C8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="102">
+      <c r="E8" s="88">
         <f>E7+E6</f>
         <v>1086</v>
       </c>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B9" s="100">
+      <c r="B9" s="19">
         <v>4</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="103">
+      <c r="E9" s="89">
         <f>'hệ số phức tạp KT-CN '!F20</f>
         <v>0.79</v>
       </c>
-      <c r="F9" s="100" t="s">
+      <c r="F9" s="19" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B10" s="100">
+      <c r="B10" s="19">
         <v>5</v>
       </c>
-      <c r="C10" s="101" t="s">
+      <c r="C10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="102">
+      <c r="E10" s="88">
         <f>'He so PTMT - KN - NOI SUY'!F29</f>
         <v>0.90499999999999992</v>
       </c>
-      <c r="F10" s="100" t="s">
+      <c r="F10" s="19" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="100">
+      <c r="B11" s="19">
         <v>6</v>
       </c>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="103">
+      <c r="E11" s="89">
         <f>E8*E9*E10</f>
         <v>776.4357</v>
       </c>
-      <c r="F11" s="100" t="s">
+      <c r="F11" s="19" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="98" t="s">
+    <row r="12" spans="2:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="99" t="s">
+      <c r="C12" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="99" t="s">
+      <c r="D12" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="106" t="str">
+      <c r="E12" s="94" t="str">
         <f>'He so PTMT - KN - NOI SUY'!G31</f>
         <v>20</v>
       </c>
-      <c r="F12" s="98" t="s">
+      <c r="F12" s="59" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="98" t="s">
+    <row r="13" spans="2:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="117">
+      <c r="E13" s="95">
         <f>10/6*E11</f>
         <v>1294.0595000000001</v>
       </c>
-      <c r="F13" s="98" t="s">
+      <c r="F13" s="59" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="98" t="s">
+    <row r="14" spans="2:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="99" t="s">
+      <c r="D14" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="118">
+      <c r="E14" s="105">
         <v>45042.307699999998</v>
       </c>
-      <c r="F14" s="98" t="s">
+      <c r="F14" s="59" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="98" t="s">
+    <row r="15" spans="2:6" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="99" t="s">
+      <c r="C15" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="119">
+      <c r="E15" s="96">
         <f>1.4*E12*E13*E14</f>
         <v>1632047933.0710282</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F15" s="59" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="95">
+      <c r="G38" s="57">
         <v>1294.06</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="95">
+      <c r="G39" s="57">
         <v>45042</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="95">
+      <c r="G40" s="57">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="95">
+      <c r="G41" s="57">
         <f>1.4* PRODUCT(G38:G40)</f>
         <v>1632037414.5599997</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="ufJuzNX6krSRLf3DNaDnVqkqJflDd4FmLPTZjMi3XR7Ywl0D3BRwdIyEVylSRWhje4HU+W6dAZy9LscxbMOFXg==" saltValue="+xpZzwxPIfjEPk9oXhr84Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3299,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCC8E97-F44B-4EAE-B5B7-A2E91844A089}">
-  <dimension ref="B3:H9"/>
+  <dimension ref="B4:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3315,113 +3143,113 @@
     <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="46" t="s">
+    <row r="4" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="78" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="78" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="78" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="50">
+    <row r="5" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="120">
+      <c r="E5" s="108">
         <f>'giá trị phần mềm'!E15</f>
         <v>1632047933.0710282</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="94"/>
-    </row>
-    <row r="6" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="47">
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24">
         <v>2</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="121">
+      <c r="E6" s="109">
         <f>E5*0.65</f>
         <v>1060831156.4961684</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="H6" s="105"/>
-    </row>
-    <row r="7" spans="2:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="47">
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="24">
         <v>3</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="122">
+      <c r="E7" s="109">
         <f>(E5+E6)*0.06</f>
         <v>161572745.37403181</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="47">
+    <row r="8" spans="2:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24">
         <v>4</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="E8" s="122">
+      <c r="E8" s="109">
         <f>SUM(E5:E7)</f>
         <v>2854451834.9412289</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="47"/>
-      <c r="C9" s="48" t="s">
+    <row r="9" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="24"/>
+      <c r="C9" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="123">
+      <c r="E9" s="97">
         <f>E8</f>
         <v>2854451834.9412289</v>
       </c>
-      <c r="F9" s="58"/>
+      <c r="F9" s="51"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="7FZN57L60QizvXf+hhlA1ebeS8Jy4CgRC4RHd8HR1GELjQOnfLwKWMqKTnLAoEwHOAeudVceh/LOvrb67q2RUg==" saltValue="Fw5UQPk/irGcOn0qAUTBrw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3431,7 +3259,7 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3442,115 +3270,115 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-    </row>
-    <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="83" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="84" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="82">
+      <c r="A5" s="65">
         <v>1</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="86">
         <v>8500000</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="87">
         <v>3</v>
       </c>
-      <c r="D5" s="85">
+      <c r="D5" s="67">
         <v>25500000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="82">
+      <c r="A6" s="65">
         <v>2</v>
       </c>
-      <c r="B6" s="83">
+      <c r="B6" s="86">
         <v>7500000</v>
       </c>
-      <c r="C6" s="84">
+      <c r="C6" s="87">
         <v>5</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="67">
         <v>37500000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="82">
+      <c r="A7" s="65">
         <v>3</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="86">
         <v>6000000</v>
       </c>
-      <c r="C7" s="84">
+      <c r="C7" s="87">
         <v>7</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="67">
         <v>45100000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="84">
+      <c r="B8" s="69"/>
+      <c r="C8" s="66">
         <f>SUM(C5:C7)</f>
         <v>15</v>
       </c>
-      <c r="D8" s="85"/>
+      <c r="D8" s="67"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="90">
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="106">
         <f>SUM(D5:D7)</f>
         <v>108100000</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="106">
         <f>D9/C8</f>
         <v>7206666.666666667</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="93">
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="107">
         <f>D10/20/8</f>
         <v>45041.666666666672</v>
       </c>
@@ -3575,7 +3403,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I18"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3667,384 +3495,384 @@
       <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="32">
         <v>1.5</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="43">
         <v>2</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="43">
         <v>2</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="43">
         <v>2</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="43">
         <v>2</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="43">
         <v>2</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="43">
         <f>AVERAGE(E4:I6)</f>
         <v>2</v>
       </c>
-      <c r="K4" s="71">
+      <c r="K4" s="40">
         <f>J4*D4</f>
         <v>3</v>
       </c>
-      <c r="L4" s="65" t="str" cm="1">
+      <c r="L4" s="32" t="str" cm="1">
         <f t="array" ref="L4">_xlfn.IFS(K4&gt;3,"1",K4&gt;2,"0.6",K4&gt;1,"0.1",K4&gt;0,"0.05",K4&lt;=0,"0")</f>
         <v>0.6</v>
       </c>
-      <c r="M4" s="65"/>
+      <c r="M4" s="32"/>
     </row>
     <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
     </row>
     <row r="7" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="32">
         <v>0.5</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="31">
         <v>3</v>
       </c>
-      <c r="F7" s="66">
+      <c r="F7" s="31">
         <v>3</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="31">
         <v>2</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="31">
         <v>2</v>
       </c>
-      <c r="I7" s="66">
+      <c r="I7" s="31">
         <v>2</v>
       </c>
-      <c r="J7" s="65">
+      <c r="J7" s="32">
         <f>AVERAGE(E7:I9)</f>
         <v>2.4</v>
       </c>
-      <c r="K7" s="71">
+      <c r="K7" s="40">
         <f>J7*D7</f>
         <v>1.2</v>
       </c>
-      <c r="L7" s="65" t="str" cm="1">
+      <c r="L7" s="32" t="str" cm="1">
         <f t="array" ref="L7">_xlfn.IFS(K7&gt;3,"1",K7&gt;2,"0.6",K7&gt;1,"0.1",K7&gt;0,"0.05",K7&lt;=0,"0")</f>
         <v>0.1</v>
       </c>
-      <c r="M7" s="66"/>
+      <c r="M7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="63"/>
-      <c r="B8" s="64"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="66"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="31"/>
     </row>
     <row r="9" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63"/>
-      <c r="B9" s="64"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="66"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="31"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="32">
         <v>1</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="31">
         <v>3</v>
       </c>
-      <c r="F10" s="66">
+      <c r="F10" s="31">
         <v>3</v>
       </c>
-      <c r="G10" s="66">
+      <c r="G10" s="31">
         <v>3</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="31">
         <v>3</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="31">
         <v>3</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="32">
         <f>AVERAGE(E10:I12)</f>
         <v>3</v>
       </c>
-      <c r="K10" s="67">
+      <c r="K10" s="33">
         <f>J10*D10</f>
         <v>3</v>
       </c>
-      <c r="L10" s="65" t="str" cm="1">
+      <c r="L10" s="32" t="str" cm="1">
         <f t="array" ref="L10">_xlfn.IFS(K10&gt;3,"1",K10&gt;2,"0.6",K10&gt;1,"0.1",K10&gt;0,"0.05",K10&lt;=0,"0")</f>
         <v>0.6</v>
       </c>
-      <c r="M10" s="66"/>
+      <c r="M10" s="31"/>
     </row>
     <row r="11" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="64"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="66"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="31"/>
     </row>
     <row r="12" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="66"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="31"/>
     </row>
     <row r="13" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="32">
         <v>0.5</v>
       </c>
-      <c r="E13" s="66">
+      <c r="E13" s="31">
         <v>3</v>
       </c>
-      <c r="F13" s="66">
+      <c r="F13" s="31">
         <v>3</v>
       </c>
-      <c r="G13" s="66">
+      <c r="G13" s="31">
         <v>1</v>
       </c>
-      <c r="H13" s="66">
+      <c r="H13" s="31">
         <v>1</v>
       </c>
-      <c r="I13" s="66">
+      <c r="I13" s="31">
         <v>1</v>
       </c>
-      <c r="J13" s="65">
+      <c r="J13" s="32">
         <f>AVERAGE(E13:I15)</f>
         <v>1.8</v>
       </c>
-      <c r="K13" s="67">
+      <c r="K13" s="33">
         <f>J13*D13</f>
         <v>0.9</v>
       </c>
-      <c r="L13" s="65" t="str" cm="1">
+      <c r="L13" s="32" t="str" cm="1">
         <f t="array" ref="L13">_xlfn.IFS(K13&gt;3,"1",K13&gt;2,"0.6",K13&gt;1,"0.1",K13&gt;0,"0.05",K13&lt;=0,"0")</f>
         <v>0.05</v>
       </c>
-      <c r="M13" s="66"/>
+      <c r="M13" s="31"/>
     </row>
     <row r="14" spans="1:13" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="66"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" spans="1:13" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="66"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="31"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="32">
         <v>1</v>
       </c>
-      <c r="E16" s="66">
+      <c r="E16" s="31">
         <v>4</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="31">
         <v>4</v>
       </c>
-      <c r="G16" s="66">
+      <c r="G16" s="31">
         <v>2</v>
       </c>
-      <c r="H16" s="66">
+      <c r="H16" s="31">
         <v>3</v>
       </c>
-      <c r="I16" s="66">
+      <c r="I16" s="31">
         <v>2</v>
       </c>
-      <c r="J16" s="65">
+      <c r="J16" s="32">
         <f>AVERAGE(E16:I18)</f>
         <v>3</v>
       </c>
-      <c r="K16" s="67">
+      <c r="K16" s="33">
         <f>J16*D16</f>
         <v>3</v>
       </c>
-      <c r="L16" s="65" t="str" cm="1">
+      <c r="L16" s="32" t="str" cm="1">
         <f t="array" ref="L16">_xlfn.IFS(K16&gt;3,"1",K16&gt;2,"0.6",K16&gt;1,"0.1",K16&gt;0,"0.05",K16&lt;=0,"0")</f>
         <v>0.6</v>
       </c>
-      <c r="M16" s="66"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="17" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="66"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="31"/>
     </row>
     <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="66"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="31"/>
     </row>
     <row r="19" spans="1:13" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
@@ -4064,55 +3892,55 @@
       <c r="M19" s="10"/>
     </row>
     <row r="20" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="35" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="32">
         <v>2</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66">
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31">
         <v>2</v>
       </c>
-      <c r="K20" s="66">
+      <c r="K20" s="31">
         <f>J20*D20</f>
         <v>4</v>
       </c>
-      <c r="L20" s="66" t="str" cm="1">
+      <c r="L20" s="31" t="str" cm="1">
         <f t="array" ref="L20">_xlfn.IFS(K20&gt;3,"1",K20&gt;2,"0.6",K20&gt;1,"0.1",K20&gt;0,"0.05",K20&lt;=0,"0")</f>
         <v>1</v>
       </c>
-      <c r="M20" s="66"/>
+      <c r="M20" s="31"/>
     </row>
     <row r="21" spans="1:13" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="65"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="66"/>
-      <c r="M21" s="66"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
     </row>
     <row r="22" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -4121,127 +3949,127 @@
       <c r="C22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="32">
         <v>-1</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="74">
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="37">
         <v>0</v>
       </c>
-      <c r="K22" s="74">
+      <c r="K22" s="37">
         <f>J22*D22</f>
         <v>0</v>
       </c>
-      <c r="L22" s="66" t="str" cm="1">
+      <c r="L22" s="31" t="str" cm="1">
         <f t="array" ref="L22">_xlfn.IFS(K22&gt;3,"1",K22&gt;2,"0.6",K22&gt;1,"0.1",K22&gt;0,"0.05",K22&lt;=0,"0")</f>
         <v>0</v>
       </c>
-      <c r="M22" s="66"/>
+      <c r="M22" s="31"/>
     </row>
     <row r="23" spans="1:13" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
     </row>
     <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="66"/>
-      <c r="M24" s="66"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
     </row>
     <row r="25" spans="1:13" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="35" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="32">
         <v>-1</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="74">
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="37">
         <v>3</v>
       </c>
-      <c r="K25" s="74">
+      <c r="K25" s="37">
         <f>J25*D25</f>
         <v>-3</v>
       </c>
-      <c r="L25" s="66" t="str" cm="1">
+      <c r="L25" s="31" t="str" cm="1">
         <f t="array" ref="L25">_xlfn.IFS(K25&gt;3,"1",K25&gt;2,"0.6",K25&gt;1,"0.1",K25&gt;0,"0.05",K25&lt;=0,"0")</f>
         <v>0</v>
       </c>
-      <c r="M25" s="66"/>
+      <c r="M25" s="31"/>
     </row>
     <row r="26" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
-      <c r="B26" s="64"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="65"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="66"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
     </row>
     <row r="27" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
-      <c r="B27" s="64"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="66"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
     </row>
     <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
@@ -4312,60 +4140,28 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="M25:M27"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="M10:M12"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="M13:M15"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="M16:M18"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="K10:K12"/>
     <mergeCell ref="A13:A15"/>
@@ -4382,31 +4178,63 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="F16:F18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
     <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="M10:M12"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="K16:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>